<commit_message>
Kit -> Recibe Fraccion y Nivel Limpieza
</commit_message>
<xml_diff>
--- a/imports/Area-SubArea.xlsx
+++ b/imports/Area-SubArea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Limpieza\LIMPIEZA_APP\sop_lavado_app\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58483BBC-A04C-4632-91A2-7667D940E117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D021054-1ACA-411F-9906-D4A9629747FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
@@ -235,9 +235,6 @@
     <t>PASILLO</t>
   </si>
   <si>
-    <t>OFCINA</t>
-  </si>
-  <si>
     <t>SALA JUNTAS</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>subarea</t>
+  </si>
+  <si>
+    <t>OFICINA</t>
   </si>
 </sst>
 </file>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1008,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>7</v>
@@ -1037,7 +1037,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="6">
         <v>4</v>
@@ -1061,7 +1061,7 @@
         <v>9</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>8</v>
@@ -1075,7 +1075,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="6">
         <v>2</v>
@@ -1099,7 +1099,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>57</v>
@@ -1113,7 +1113,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1145,7 +1145,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="6">
         <v>2</v>
@@ -1177,7 +1177,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="6">
         <v>7</v>
@@ -1209,7 +1209,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -1241,7 +1241,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1392,13 +1392,13 @@
         <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>7</v>
@@ -1430,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>27</v>
@@ -1460,13 +1460,13 @@
         <v>9</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>8</v>
@@ -1480,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>27</v>
@@ -1510,13 +1510,13 @@
         <v>12</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>57</v>
@@ -1530,7 +1530,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>27</v>
@@ -1574,7 +1574,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>27</v>
@@ -1604,7 +1604,7 @@
         <v>16</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>16</v>
@@ -1618,7 +1618,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>27</v>
@@ -1648,7 +1648,7 @@
         <v>42</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>18</v>
@@ -1662,7 +1662,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>27</v>
@@ -1706,7 +1706,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>27</v>
@@ -1746,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>27</v>
@@ -1778,7 +1778,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>27</v>
@@ -1810,7 +1810,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>27</v>
@@ -1842,7 +1842,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>27</v>
@@ -1874,7 +1874,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>27</v>
@@ -1906,7 +1906,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>27</v>
@@ -1938,7 +1938,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>27</v>
@@ -1970,7 +1970,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>27</v>
@@ -2002,7 +2002,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>27</v>
@@ -2034,7 +2034,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>27</v>
@@ -2066,7 +2066,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>27</v>
@@ -2098,7 +2098,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>27</v>

</xml_diff>